<commit_message>
Test Asmita over Holocene and modified WaterLevels to provide correct input and sealevelrise.m to handle the pivotyear correctly. Adjusted AsmitaModel.m to use durations if StartYear<0 and datetime otherwise. Corrected spelling of 'been' in AsmitaModel.m Added trap for incorrect matrix dimensions in Advection. Added trap for mismatch between Element and Interventions array dimensions. Corrected AsmitaModel.CheckInputso that river mass balance does not overwrite ok when other checks have set ok=0.
Updated instructions and slides to clarify task
Added slides on workflow and how to add river input

Added trap in wave_cco_format.m to handle users who are not using UK Locale
Added lambertw function to coastal functions folder and updated help (svn version)
Added lambertw function to estuary functions folder and updated help


git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@89 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/SW4e model parameters.xlsx
+++ b/Training exercise/SW4e model parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Tools\MATLAB\AsmitaOO\Training exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Tools\MATLAB\MUImodels2\muiApps\Asmita\Training exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEB6FDE-C179-421E-90B8-7980B5483C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0004FFA-D214-4DF5-8D78-E3F7BBD02D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="21600" windowHeight="11422" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
   <si>
     <t>concentration imported by advection (kg/m^3)</t>
   </si>
@@ -204,9 +204,6 @@
     <t xml:space="preserve"> Intertidal exchange coeff, di=Di*tr/2*Lr/wi</t>
   </si>
   <si>
-    <t>Global equilbirium concentration (kg/m^3)</t>
-  </si>
-  <si>
     <t>Historic changes in volume and area within Southampton Water</t>
   </si>
   <si>
@@ -283,6 +280,15 @@
   </si>
   <si>
     <t>area</t>
+  </si>
+  <si>
+    <t>Global equilibrium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Flow input and Equilibrium concentrations (kg/m^3)</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -435,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,6 +706,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1052,34 +1061,34 @@
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.265625" customWidth="1"/>
-    <col min="2" max="2" width="16.73046875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.59765625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.73046875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.59765625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="15.86328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.86328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1328125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="12.86328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.265625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="11.1328125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="24.265625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="11.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6328125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.08984375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="11.08984375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="24.26953125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="11.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1095,10 +1104,10 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>29</v>
       </c>
@@ -1126,21 +1135,21 @@
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="13.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>78</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>79</v>
       </c>
       <c r="F4" s="46"/>
       <c r="G4" s="16"/>
@@ -1154,7 +1163,7 @@
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
     </row>
-    <row r="5" spans="1:16" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>32</v>
       </c>
@@ -1185,7 +1194,7 @@
       <c r="O5" s="31"/>
       <c r="P5" s="31"/>
     </row>
-    <row r="6" spans="1:16" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
         <v>33</v>
       </c>
@@ -1216,7 +1225,7 @@
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
     </row>
-    <row r="7" spans="1:16" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
         <v>34</v>
       </c>
@@ -1244,7 +1253,7 @@
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
     </row>
-    <row r="8" spans="1:16" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>35</v>
       </c>
@@ -1272,7 +1281,7 @@
       <c r="O8" s="31"/>
       <c r="P8" s="31"/>
     </row>
-    <row r="9" spans="1:16" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="68" t="s">
         <v>36</v>
       </c>
@@ -1300,7 +1309,7 @@
       <c r="O9" s="70"/>
       <c r="P9" s="70"/>
     </row>
-    <row r="10" spans="1:16" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>37</v>
       </c>
@@ -1328,7 +1337,7 @@
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
     </row>
-    <row r="11" spans="1:16" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72" t="s">
         <v>38</v>
       </c>
@@ -1356,7 +1365,7 @@
       <c r="O11" s="70"/>
       <c r="P11" s="70"/>
     </row>
-    <row r="12" spans="1:16" s="38" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="73" t="s">
         <v>39</v>
       </c>
@@ -1381,7 +1390,7 @@
       <c r="L12" s="74"/>
       <c r="M12" s="74"/>
     </row>
-    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
         <v>40</v>
       </c>
@@ -1408,7 +1417,7 @@
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:16" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="47" t="s">
         <v>41</v>
       </c>
@@ -1436,7 +1445,7 @@
       <c r="O14"/>
       <c r="P14"/>
     </row>
-    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="47" t="s">
         <v>42</v>
       </c>
@@ -1463,7 +1472,7 @@
       <c r="N15"/>
       <c r="O15"/>
     </row>
-    <row r="16" spans="1:16" s="38" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="73" t="s">
         <v>31</v>
       </c>
@@ -1488,7 +1497,7 @@
       <c r="L16" s="76"/>
       <c r="M16" s="76"/>
     </row>
-    <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
@@ -1517,7 +1526,7 @@
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>44</v>
       </c>
@@ -1548,7 +1557,7 @@
       <c r="N18"/>
       <c r="O18"/>
     </row>
-    <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
@@ -1575,9 +1584,9 @@
       <c r="N19"/>
       <c r="O19"/>
     </row>
-    <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="33">
         <v>0</v>
@@ -1591,7 +1600,9 @@
       <c r="E20" s="33">
         <v>0</v>
       </c>
-      <c r="F20" s="33"/>
+      <c r="F20" s="33" t="s">
+        <v>82</v>
+      </c>
       <c r="G20" s="48"/>
       <c r="H20" s="33"/>
       <c r="I20" s="33"/>
@@ -1602,9 +1613,9 @@
       <c r="N20"/>
       <c r="O20"/>
     </row>
-    <row r="21" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="87" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="B21" s="88" t="s">
         <v>6</v>
@@ -1612,8 +1623,8 @@
       <c r="C21" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="88" t="s">
-        <v>6</v>
+      <c r="D21" s="105">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E21" s="88" t="s">
         <v>6</v>
@@ -1631,7 +1642,7 @@
       <c r="N21"/>
       <c r="O21"/>
     </row>
-    <row r="22" spans="1:16" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="67" t="s">
         <v>46</v>
       </c>
@@ -1660,7 +1671,7 @@
       <c r="L22" s="39"/>
       <c r="M22" s="39"/>
     </row>
-    <row r="23" spans="1:16" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="67" t="s">
         <v>47</v>
       </c>
@@ -1687,7 +1698,7 @@
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
     </row>
-    <row r="24" spans="1:16" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="67" t="s">
         <v>48</v>
       </c>
@@ -1716,7 +1727,7 @@
       <c r="L24" s="42"/>
       <c r="M24" s="42"/>
     </row>
-    <row r="25" spans="1:16" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="67" t="s">
         <v>49</v>
       </c>
@@ -1745,7 +1756,7 @@
       <c r="L25" s="42"/>
       <c r="M25" s="42"/>
     </row>
-    <row r="26" spans="1:16" s="60" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="81" t="s">
         <v>50</v>
       </c>
@@ -1774,7 +1785,7 @@
       <c r="L26" s="82"/>
       <c r="M26" s="82"/>
     </row>
-    <row r="27" spans="1:16" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="67" t="s">
         <v>51</v>
       </c>
@@ -1801,7 +1812,7 @@
       <c r="L27" s="42"/>
       <c r="M27" s="42"/>
     </row>
-    <row r="28" spans="1:16" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="67" t="s">
         <v>52</v>
       </c>
@@ -1828,7 +1839,7 @@
       <c r="L28" s="42"/>
       <c r="M28" s="42"/>
     </row>
-    <row r="29" spans="1:16" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="67" t="s">
         <v>53</v>
       </c>
@@ -1855,7 +1866,7 @@
       <c r="L29" s="44"/>
       <c r="M29" s="44"/>
     </row>
-    <row r="30" spans="1:16" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="67" t="s">
         <v>54</v>
       </c>
@@ -1882,7 +1893,7 @@
       <c r="L30" s="44"/>
       <c r="M30" s="44"/>
     </row>
-    <row r="31" spans="1:16" s="60" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="81" t="s">
         <v>55</v>
       </c>
@@ -1909,7 +1920,7 @@
       <c r="L31" s="86"/>
       <c r="M31" s="86"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B32" s="8"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -1921,7 +1932,7 @@
       <c r="O32" s="12"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -1930,7 +1941,7 @@
       <c r="M33" s="15"/>
       <c r="P33" s="14"/>
     </row>
-    <row r="34" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1946,34 +1957,34 @@
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" s="5">
         <v>6.1</v>
       </c>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B37" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B38" s="5">
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" s="5">
         <v>2650</v>
       </c>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" s="10">
         <v>2E-3</v>
       </c>
@@ -1981,33 +1992,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="53"/>
       <c r="B45" s="52"/>
       <c r="C45" s="52"/>
       <c r="D45" s="52"/>
     </row>
-    <row r="46" spans="1:17" s="60" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:17" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="54" t="s">
         <v>9</v>
       </c>
@@ -2032,7 +2043,7 @@
       <c r="N46" s="59"/>
       <c r="O46" s="59"/>
     </row>
-    <row r="47" spans="1:17" s="60" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:17" s="60" customFormat="1" ht="100" x14ac:dyDescent="0.3">
       <c r="A47" s="61" t="s">
         <v>10</v>
       </c>
@@ -2057,7 +2068,7 @@
       <c r="N47" s="59"/>
       <c r="O47" s="59"/>
     </row>
-    <row r="48" spans="1:17" s="60" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:17" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="64" t="s">
         <v>13</v>
       </c>
@@ -2077,7 +2088,7 @@
       <c r="N48" s="59"/>
       <c r="O48" s="59"/>
     </row>
-    <row r="49" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="64" t="s">
         <v>16</v>
       </c>
@@ -2098,7 +2109,7 @@
       <c r="N49" s="59"/>
       <c r="O49" s="59"/>
     </row>
-    <row r="50" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="64" t="s">
         <v>17</v>
       </c>
@@ -2119,7 +2130,7 @@
       <c r="N50" s="59"/>
       <c r="O50" s="59"/>
     </row>
-    <row r="51" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="64" t="s">
         <v>3</v>
       </c>
@@ -2139,7 +2150,7 @@
       <c r="N51" s="59"/>
       <c r="O51" s="59"/>
     </row>
-    <row r="52" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="64" t="s">
         <v>4</v>
       </c>
@@ -2159,7 +2170,7 @@
       <c r="N52" s="59"/>
       <c r="O52" s="59"/>
     </row>
-    <row r="53" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="64" t="s">
         <v>5</v>
       </c>
@@ -2179,7 +2190,7 @@
       <c r="N53" s="59"/>
       <c r="O53" s="59"/>
     </row>
-    <row r="54" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="64" t="s">
         <v>24</v>
       </c>
@@ -2200,7 +2211,7 @@
       <c r="N54" s="59"/>
       <c r="O54" s="59"/>
     </row>
-    <row r="55" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="64" t="s">
         <v>0</v>
       </c>
@@ -2221,7 +2232,7 @@
       <c r="N55" s="59"/>
       <c r="O55" s="59"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F56" s="20"/>
       <c r="G56" s="20"/>
       <c r="H56" s="20"/>
@@ -2229,7 +2240,7 @@
       <c r="J56" s="20"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F57" s="21"/>
       <c r="G57" s="21"/>
       <c r="H57" s="21"/>
@@ -2250,33 +2261,33 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="A6:E80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" style="93" customWidth="1"/>
-    <col min="3" max="3" width="12.73046875" style="96" customWidth="1"/>
-    <col min="4" max="4" width="12.73046875" style="93" customWidth="1"/>
-    <col min="5" max="5" width="12.73046875" style="96" customWidth="1"/>
-    <col min="6" max="6" width="12.73046875" style="93" customWidth="1"/>
-    <col min="7" max="7" width="12.73046875" style="96" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="93" customWidth="1"/>
-    <col min="9" max="9" width="12.73046875" style="96" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="93" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="96" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="93" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="96" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" style="93" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="96" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="93" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" style="96" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="99" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" s="99" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="97" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="98"/>
       <c r="C1" s="98"/>
@@ -2286,9 +2297,9 @@
       <c r="G1" s="98"/>
       <c r="H1" s="98"/>
     </row>
-    <row r="2" spans="1:22" s="99" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" s="99" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="100" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="98"/>
       <c r="C2" s="98"/>
@@ -2298,84 +2309,84 @@
       <c r="G2" s="98"/>
       <c r="H2" s="98"/>
     </row>
-    <row r="3" spans="1:22" s="91" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:22" s="91" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="90" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="105" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="106" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105" t="s">
+      <c r="E3" s="106"/>
+      <c r="F3" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105" t="s">
+      <c r="G3" s="106"/>
+      <c r="H3" s="106" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="105"/>
-    </row>
-    <row r="4" spans="1:22" s="91" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="106"/>
+    </row>
+    <row r="4" spans="1:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="102"/>
       <c r="B4" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="D4" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="94" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="94" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="94" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="101" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="94" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="94" t="s">
+      <c r="C5" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="94" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="94" t="s">
+      <c r="D5" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="94" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" s="94" t="s">
+      <c r="E5" s="94" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" s="91" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="101" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="94" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="94" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="94" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="94" t="s">
-        <v>66</v>
-      </c>
       <c r="F5" s="94" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="94" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H5" s="94" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" s="94" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="101">
         <v>1926</v>
       </c>
@@ -2394,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="101">
         <v>1927</v>
       </c>
@@ -2412,7 +2423,7 @@
         <v>-667500</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="101">
         <v>1928</v>
       </c>
@@ -2424,7 +2435,7 @@
       <c r="F8" s="92"/>
       <c r="G8" s="95"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="101">
         <v>1929</v>
       </c>
@@ -2436,7 +2447,7 @@
       <c r="F9" s="92"/>
       <c r="G9" s="95"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="101">
         <v>1930</v>
       </c>
@@ -2444,7 +2455,7 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="101">
         <v>1931</v>
       </c>
@@ -2462,7 +2473,7 @@
       </c>
       <c r="N11" s="28"/>
     </row>
-    <row r="12" spans="1:22" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="101">
         <v>1932</v>
       </c>
@@ -2480,7 +2491,7 @@
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
     </row>
-    <row r="13" spans="1:22" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="101">
         <v>1933</v>
       </c>
@@ -2498,7 +2509,7 @@
       <c r="U13" s="19"/>
       <c r="V13" s="19"/>
     </row>
-    <row r="14" spans="1:22" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="101">
         <v>1934</v>
       </c>
@@ -2515,7 +2526,7 @@
       <c r="T14" s="9"/>
       <c r="U14" s="9"/>
     </row>
-    <row r="15" spans="1:22" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="101">
         <v>1935</v>
       </c>
@@ -2532,7 +2543,7 @@
       <c r="T15" s="9"/>
       <c r="U15" s="9"/>
     </row>
-    <row r="16" spans="1:22" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="101">
         <v>1936</v>
       </c>
@@ -2549,7 +2560,7 @@
       <c r="T16" s="9"/>
       <c r="U16" s="9"/>
     </row>
-    <row r="17" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="101">
         <v>1937</v>
       </c>
@@ -2566,7 +2577,7 @@
       <c r="T17" s="9"/>
       <c r="U17" s="9"/>
     </row>
-    <row r="18" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="101">
         <v>1938</v>
       </c>
@@ -2586,7 +2597,7 @@
       <c r="T18" s="9"/>
       <c r="U18" s="9"/>
     </row>
-    <row r="19" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="101">
         <v>1939</v>
       </c>
@@ -2603,7 +2614,7 @@
       <c r="T19" s="9"/>
       <c r="U19" s="9"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="101">
         <v>1940</v>
       </c>
@@ -2612,7 +2623,7 @@
       </c>
       <c r="N20" s="29"/>
     </row>
-    <row r="21" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="101">
         <v>1941</v>
       </c>
@@ -2628,7 +2639,7 @@
       <c r="S21" s="23"/>
       <c r="T21" s="5"/>
     </row>
-    <row r="22" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="101">
         <v>1942</v>
       </c>
@@ -2644,7 +2655,7 @@
       <c r="S22" s="25"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="101">
         <v>1943</v>
       </c>
@@ -2660,7 +2671,7 @@
       <c r="S23" s="25"/>
       <c r="T23" s="5"/>
     </row>
-    <row r="24" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="101">
         <v>1944</v>
       </c>
@@ -2676,7 +2687,7 @@
       <c r="S24" s="25"/>
       <c r="T24" s="5"/>
     </row>
-    <row r="25" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="101">
         <v>1945</v>
       </c>
@@ -2692,7 +2703,7 @@
       <c r="S25" s="25"/>
       <c r="T25" s="5"/>
     </row>
-    <row r="26" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="101">
         <v>1946</v>
       </c>
@@ -2708,7 +2719,7 @@
       <c r="S26" s="25"/>
       <c r="T26" s="5"/>
     </row>
-    <row r="27" spans="1:21" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="101">
         <v>1947</v>
       </c>
@@ -2724,7 +2735,7 @@
       <c r="S27" s="25"/>
       <c r="T27" s="5"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="101">
         <v>1948</v>
       </c>
@@ -2732,7 +2743,7 @@
         <v>370000</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="101">
         <v>1949</v>
       </c>
@@ -2740,7 +2751,7 @@
         <v>370000</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="101">
         <v>1950</v>
       </c>
@@ -2748,7 +2759,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="101">
         <v>1951</v>
       </c>
@@ -2756,7 +2767,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="101">
         <v>1952</v>
       </c>
@@ -2764,7 +2775,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="101">
         <v>1953</v>
       </c>
@@ -2772,7 +2783,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="101">
         <v>1954</v>
       </c>
@@ -2781,7 +2792,7 @@
       </c>
       <c r="N34" s="11"/>
     </row>
-    <row r="35" spans="1:14" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A35" s="101">
         <v>1955</v>
       </c>
@@ -2790,7 +2801,7 @@
       </c>
       <c r="N35" s="11"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="101">
         <v>1956</v>
       </c>
@@ -2798,7 +2809,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="101">
         <v>1957</v>
       </c>
@@ -2806,7 +2817,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A38" s="101">
         <v>1958</v>
       </c>
@@ -2814,7 +2825,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A39" s="101">
         <v>1959</v>
       </c>
@@ -2822,7 +2833,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A40" s="101">
         <v>1960</v>
       </c>
@@ -2830,7 +2841,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A41" s="101">
         <v>1961</v>
       </c>
@@ -2844,7 +2855,7 @@
         <v>-412500</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A42" s="101">
         <v>1962</v>
       </c>
@@ -2852,7 +2863,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A43" s="101">
         <v>1963</v>
       </c>
@@ -2860,7 +2871,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A44" s="101">
         <v>1964</v>
       </c>
@@ -2868,7 +2879,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="101">
         <v>1965</v>
       </c>
@@ -2897,7 +2908,7 @@
         <v>-1371379</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A46" s="101">
         <v>1966</v>
       </c>
@@ -2905,7 +2916,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A47" s="101">
         <v>1967</v>
       </c>
@@ -2913,7 +2924,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A48" s="101">
         <v>1968</v>
       </c>
@@ -2921,7 +2932,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A49" s="101">
         <v>1969</v>
       </c>
@@ -2929,7 +2940,7 @@
         <v>780000</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A50" s="101">
         <v>1970</v>
       </c>
@@ -2937,7 +2948,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A51" s="101">
         <v>1971</v>
       </c>
@@ -2945,7 +2956,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A52" s="101">
         <v>1972</v>
       </c>
@@ -2953,7 +2964,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A53" s="101">
         <v>1973</v>
       </c>
@@ -2961,7 +2972,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A54" s="101">
         <v>1974</v>
       </c>
@@ -2969,7 +2980,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A55" s="101">
         <v>1975</v>
       </c>
@@ -2977,7 +2988,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A56" s="101">
         <v>1976</v>
       </c>
@@ -2985,7 +2996,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A57" s="101">
         <v>1977</v>
       </c>
@@ -2993,7 +3004,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A58" s="101">
         <v>1978</v>
       </c>
@@ -3001,7 +3012,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A59" s="101">
         <v>1979</v>
       </c>
@@ -3009,7 +3020,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A60" s="101">
         <v>1980</v>
       </c>
@@ -3017,7 +3028,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A61" s="101">
         <v>1981</v>
       </c>
@@ -3025,7 +3036,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A62" s="101">
         <v>1982</v>
       </c>
@@ -3033,7 +3044,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A63" s="101">
         <v>1983</v>
       </c>
@@ -3041,7 +3052,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A64" s="101">
         <v>1984</v>
       </c>
@@ -3049,7 +3060,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A65" s="101">
         <v>1985</v>
       </c>
@@ -3057,7 +3068,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A66" s="101">
         <v>1986</v>
       </c>
@@ -3065,7 +3076,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A67" s="101">
         <v>1987</v>
       </c>
@@ -3073,7 +3084,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A68" s="101">
         <v>1988</v>
       </c>
@@ -3081,7 +3092,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A69" s="101">
         <v>1989</v>
       </c>
@@ -3089,7 +3100,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A70" s="101">
         <v>1990</v>
       </c>
@@ -3097,7 +3108,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A71" s="101">
         <v>1991</v>
       </c>
@@ -3105,7 +3116,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A72" s="101">
         <v>1992</v>
       </c>
@@ -3113,7 +3124,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A73" s="101">
         <v>1993</v>
       </c>
@@ -3121,7 +3132,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A74" s="101">
         <v>1994</v>
       </c>
@@ -3129,7 +3140,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="101">
         <v>1995</v>
       </c>
@@ -3140,7 +3151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A76" s="101">
         <v>1996</v>
       </c>
@@ -3148,7 +3159,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A77" s="101">
         <v>1997</v>
       </c>
@@ -3156,7 +3167,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="101">
         <v>1998</v>
       </c>
@@ -3167,7 +3178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A79" s="101">
         <v>1999</v>
       </c>
@@ -3175,7 +3186,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A80" s="101">
         <v>2000</v>
       </c>
@@ -3201,24 +3212,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1926</v>
       </c>
@@ -3229,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1927</v>
       </c>
@@ -3240,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1928</v>
       </c>
@@ -3251,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1929</v>
       </c>
@@ -3262,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1930</v>
       </c>
@@ -3273,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1931</v>
       </c>
@@ -3284,7 +3295,7 @@
         <v>710743</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1932</v>
       </c>
@@ -3295,7 +3306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1933</v>
       </c>
@@ -3306,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1934</v>
       </c>
@@ -3317,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1935</v>
       </c>
@@ -3328,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1936</v>
       </c>
@@ -3339,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1937</v>
       </c>
@@ -3350,7 +3361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1938</v>
       </c>
@@ -3361,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1939</v>
       </c>
@@ -3372,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1940</v>
       </c>
@@ -3383,7 +3394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1941</v>
       </c>
@@ -3394,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1942</v>
       </c>
@@ -3405,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1943</v>
       </c>
@@ -3416,7 +3427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1944</v>
       </c>
@@ -3427,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1945</v>
       </c>
@@ -3438,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1946</v>
       </c>
@@ -3449,7 +3460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1947</v>
       </c>
@@ -3460,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1948</v>
       </c>
@@ -3471,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1949</v>
       </c>
@@ -3482,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1950</v>
       </c>
@@ -3493,7 +3504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1951</v>
       </c>
@@ -3504,7 +3515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1952</v>
       </c>
@@ -3515,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1953</v>
       </c>
@@ -3526,7 +3537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1954</v>
       </c>
@@ -3537,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1955</v>
       </c>
@@ -3548,7 +3559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1956</v>
       </c>
@@ -3559,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1957</v>
       </c>
@@ -3570,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1958</v>
       </c>
@@ -3581,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1959</v>
       </c>
@@ -3592,7 +3603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1960</v>
       </c>
@@ -3603,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1961</v>
       </c>
@@ -3614,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1962</v>
       </c>
@@ -3625,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1963</v>
       </c>
@@ -3636,7 +3647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1964</v>
       </c>
@@ -3647,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1965</v>
       </c>
@@ -3658,7 +3669,7 @@
         <v>343245</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1966</v>
       </c>
@@ -3669,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1967</v>
       </c>
@@ -3680,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1968</v>
       </c>
@@ -3691,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1969</v>
       </c>
@@ -3702,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1970</v>
       </c>
@@ -3713,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1971</v>
       </c>
@@ -3724,7 +3735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1972</v>
       </c>
@@ -3735,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1973</v>
       </c>
@@ -3746,7 +3757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1974</v>
       </c>
@@ -3757,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1975</v>
       </c>
@@ -3768,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1976</v>
       </c>
@@ -3779,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1977</v>
       </c>
@@ -3790,7 +3801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1978</v>
       </c>
@@ -3801,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1979</v>
       </c>
@@ -3812,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1980</v>
       </c>
@@ -3823,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1981</v>
       </c>
@@ -3834,7 +3845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1982</v>
       </c>
@@ -3845,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1983</v>
       </c>
@@ -3856,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1984</v>
       </c>
@@ -3867,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1985</v>
       </c>
@@ -3878,7 +3889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1986</v>
       </c>
@@ -3889,7 +3900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1987</v>
       </c>
@@ -3900,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1988</v>
       </c>
@@ -3911,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1989</v>
       </c>
@@ -3922,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1990</v>
       </c>
@@ -3933,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1991</v>
       </c>
@@ -3944,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1992</v>
       </c>
@@ -3955,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1993</v>
       </c>
@@ -3966,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1994</v>
       </c>
@@ -3977,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1995</v>
       </c>
@@ -3988,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1996</v>
       </c>
@@ -3999,7 +4010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1997</v>
       </c>
@@ -4010,7 +4021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1998</v>
       </c>
@@ -4021,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1999</v>
       </c>
@@ -4032,7 +4043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2000</v>
       </c>
@@ -4043,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2001</v>
       </c>
@@ -4054,7 +4065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2002</v>
       </c>
@@ -4065,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2003</v>
       </c>
@@ -4076,7 +4087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2004</v>
       </c>
@@ -4087,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2005</v>
       </c>
@@ -4098,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2006</v>
       </c>
@@ -4109,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2007</v>
       </c>
@@ -4120,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2008</v>
       </c>
@@ -4131,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2009</v>
       </c>
@@ -4142,7 +4153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2010</v>
       </c>
@@ -4153,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2011</v>
       </c>
@@ -4164,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2012</v>
       </c>
@@ -4175,7 +4186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2013</v>
       </c>
@@ -4186,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2014</v>
       </c>
@@ -4197,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2015</v>
       </c>
@@ -4208,7 +4219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2016</v>
       </c>
@@ -4219,7 +4230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2017</v>
       </c>
@@ -4230,7 +4241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2018</v>
       </c>
@@ -4241,7 +4252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2019</v>
       </c>
@@ -4252,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2020</v>
       </c>
@@ -4263,7 +4274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2021</v>
       </c>
@@ -4274,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2022</v>
       </c>
@@ -4285,7 +4296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2023</v>
       </c>
@@ -4296,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -4307,7 +4318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2025</v>
       </c>
@@ -4318,7 +4329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2026</v>
       </c>
@@ -4329,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2027</v>
       </c>
@@ -4340,7 +4351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2028</v>
       </c>
@@ -4351,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2029</v>
       </c>
@@ -4362,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2030</v>
       </c>
@@ -4373,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2031</v>
       </c>
@@ -4384,7 +4395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2032</v>
       </c>
@@ -4395,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2033</v>
       </c>
@@ -4406,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2034</v>
       </c>
@@ -4417,7 +4428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2035</v>
       </c>
@@ -4428,7 +4439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2036</v>
       </c>
@@ -4439,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2037</v>
       </c>
@@ -4450,7 +4461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2038</v>
       </c>
@@ -4461,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2039</v>
       </c>
@@ -4472,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2040</v>
       </c>
@@ -4483,7 +4494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2041</v>
       </c>
@@ -4494,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2042</v>
       </c>
@@ -4505,7 +4516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2043</v>
       </c>
@@ -4516,7 +4527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2044</v>
       </c>
@@ -4527,7 +4538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2045</v>
       </c>
@@ -4538,7 +4549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2046</v>
       </c>
@@ -4549,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2047</v>
       </c>
@@ -4560,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2048</v>
       </c>
@@ -4571,7 +4582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2049</v>
       </c>
@@ -4582,7 +4593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2050</v>
       </c>
@@ -4593,7 +4604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2051</v>
       </c>
@@ -4604,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2052</v>
       </c>
@@ -4615,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2053</v>
       </c>
@@ -4626,7 +4637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2054</v>
       </c>
@@ -4637,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2055</v>
       </c>
@@ -4648,7 +4659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2056</v>
       </c>
@@ -4659,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2057</v>
       </c>
@@ -4670,7 +4681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2058</v>
       </c>
@@ -4681,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2059</v>
       </c>
@@ -4692,7 +4703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2060</v>
       </c>
@@ -4703,7 +4714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2061</v>
       </c>
@@ -4714,7 +4725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2062</v>
       </c>
@@ -4725,7 +4736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2063</v>
       </c>
@@ -4736,7 +4747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2064</v>
       </c>
@@ -4747,7 +4758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2065</v>
       </c>
@@ -4758,7 +4769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2066</v>
       </c>
@@ -4769,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2067</v>
       </c>
@@ -4780,7 +4791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2068</v>
       </c>
@@ -4791,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2069</v>
       </c>
@@ -4802,7 +4813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2070</v>
       </c>
@@ -4813,7 +4824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2071</v>
       </c>
@@ -4824,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2072</v>
       </c>
@@ -4835,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2073</v>
       </c>
@@ -4846,7 +4857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2074</v>
       </c>
@@ -4857,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2075</v>
       </c>
@@ -4868,7 +4879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2076</v>
       </c>
@@ -4879,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2077</v>
       </c>
@@ -4890,7 +4901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2078</v>
       </c>
@@ -4901,7 +4912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2079</v>
       </c>
@@ -4912,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2080</v>
       </c>
@@ -4923,7 +4934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2081</v>
       </c>
@@ -4934,7 +4945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2082</v>
       </c>
@@ -4945,7 +4956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2083</v>
       </c>
@@ -4956,7 +4967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2084</v>
       </c>
@@ -4967,7 +4978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>2085</v>
       </c>
@@ -4978,7 +4989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2086</v>
       </c>
@@ -4989,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2087</v>
       </c>
@@ -5000,7 +5011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2088</v>
       </c>
@@ -5011,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2089</v>
       </c>
@@ -5022,7 +5033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2090</v>
       </c>
@@ -5033,7 +5044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2091</v>
       </c>
@@ -5044,7 +5055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2092</v>
       </c>
@@ -5055,7 +5066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2093</v>
       </c>
@@ -5066,7 +5077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2094</v>
       </c>
@@ -5077,7 +5088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2095</v>
       </c>
@@ -5088,7 +5099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>2096</v>
       </c>
@@ -5099,7 +5110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2097</v>
       </c>
@@ -5110,7 +5121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2098</v>
       </c>
@@ -5121,7 +5132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2099</v>
       </c>
@@ -5132,7 +5143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2100</v>
       </c>
@@ -5150,151 +5161,166 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="A2:H5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.73046875" customWidth="1"/>
-    <col min="2" max="2" width="14.1328125" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" customWidth="1"/>
-    <col min="5" max="5" width="17.265625" customWidth="1"/>
-    <col min="6" max="6" width="12.3984375" customWidth="1"/>
-    <col min="7" max="7" width="13.59765625" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="30">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30">
         <v>17640829</v>
       </c>
-      <c r="B2" s="30">
+      <c r="C2" s="30">
         <v>16173938</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>10000</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1650</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="30">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="30">
         <v>12195117</v>
       </c>
-      <c r="B3" s="30">
+      <c r="C3" s="30">
         <v>5114469</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>8000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1650</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="30">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="30">
         <v>23242981</v>
       </c>
-      <c r="B4" s="30">
+      <c r="C4" s="30">
         <v>8098773</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>10000</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1350</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="30">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="30">
         <v>8606397</v>
       </c>
-      <c r="B5" s="30">
+      <c r="C5" s="30">
         <v>4996155</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>8000</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1350</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Asmita Fixed issued in Interventions.selectIntElement where a check statement was incomplete and needed ~isempty(obj) to be added Advection - delEleAdvection and setAdvectionProps modified to reassign advections and array dimensions correctly when deleting elements taking account of flowpath. Element - Changed order in which components are deleted in delElement. Estuary - simialr change to delEleDispersion to reassign dispersion input when deleting elements.
Added SpitDeltaSEM and WaveRayModel Apps folders




git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@132 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/SW4e model parameters.xlsx
+++ b/Training exercise/SW4e model parameters.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Tools\MATLAB\MUImodels2\muiApps\Asmita\Training exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0004FFA-D214-4DF5-8D78-E3F7BBD02D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDEA1F5-5893-48CA-A7CA-5DC9507F5D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24630" yWindow="880" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Readme" sheetId="1" r:id="rId1"/>
+    <sheet name="Inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Changes" sheetId="2" r:id="rId2"/>
     <sheet name="Change Summary" sheetId="4" r:id="rId3"/>
     <sheet name="Load" sheetId="3" r:id="rId4"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
   <si>
     <t>concentration imported by advection (kg/m^3)</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Volume</t>
   </si>
   <si>
-    <t>For a delta this is either the volume of sand above the surrounding bed level or the volume of water over the delta (latter preferred)</t>
-  </si>
-  <si>
     <t>The volume of water over the tidal flats between high and low water</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>The surface area enclosing the volumes of each element</t>
   </si>
   <si>
-    <t>This is the side slope of the channel at low water and of the flat and marsh elements at high water (not needed for delta)</t>
-  </si>
-  <si>
-    <t>Transverse slope</t>
-  </si>
-  <si>
     <t>Length of element</t>
   </si>
   <si>
@@ -159,12 +150,6 @@
     <t xml:space="preserve"> Vertical exchange, ws (m/s)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Volume Equilibrium Coefficient, kVp</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Surface Area Equilibrium Coefficient, kSp</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Peak flow velocity in element, u</t>
   </si>
   <si>
@@ -258,9 +243,6 @@
     <t>TidalDamping</t>
   </si>
   <si>
-    <t xml:space="preserve"> Flow rate of advective inputs, eg river flows (m3/s)</t>
-  </si>
-  <si>
     <t>SW (outer) channel</t>
   </si>
   <si>
@@ -282,13 +264,85 @@
     <t>area</t>
   </si>
   <si>
-    <t>Global equilibrium</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Flow input and Equilibrium concentrations (kg/m^3)</t>
-  </si>
-  <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mean sea level at t=0 (mOD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rate of sea level change (m/year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Number of cycles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amplitude of cycle (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Period of cycle (years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phase of cycle (years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LW/HW factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Coarse equilibrium concentration (kg/m^3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fine equilibrium concentration (kg/m^3)</t>
+  </si>
+  <si>
+    <t>Run time variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Size of time-step in computation (years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Number of time-steps to be considered (-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start year (years AD)</t>
+  </si>
+  <si>
+    <t>Advective exchange (river and drift)</t>
+  </si>
+  <si>
+    <t>River flow rate (m3/s)</t>
+  </si>
+  <si>
+    <t>River sediment concentration</t>
+  </si>
+  <si>
+    <t>For a delta this is usually taken as the volume of sand above the surrounding bed level (hence -ve n value)</t>
+  </si>
+  <si>
+    <t>Hydraulic parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tidal amplitude (m)</t>
+  </si>
+  <si>
+    <t>System parameters</t>
+  </si>
+  <si>
+    <t>Area e-folding convergence length (m)</t>
+  </si>
+  <si>
+    <t>Wind speed (m/s)</t>
+  </si>
+  <si>
+    <t>Wind elevation (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eq. volume scaling coefficient, alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eq. volume shape coefficient, beta</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -441,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,7 +519,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -476,7 +530,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -524,7 +578,7 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -543,7 +597,7 @@
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -558,10 +612,6 @@
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -571,7 +621,7 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -602,9 +652,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -668,15 +715,6 @@
     <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -688,14 +726,10 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -706,11 +740,25 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1058,14 +1106,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1108,20 +1156,20 @@
       <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
-        <v>29</v>
+      <c r="A3" s="46" t="s">
+        <v>26</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -1136,22 +1184,24 @@
       <c r="P3" s="16"/>
     </row>
     <row r="4" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="47" t="s">
-        <v>30</v>
+      <c r="A4" s="46" t="s">
+        <v>27</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="46"/>
+        <v>72</v>
+      </c>
+      <c r="F4" s="103" t="s">
+        <v>102</v>
+      </c>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -1164,8 +1214,8 @@
       <c r="P4" s="22"/>
     </row>
     <row r="5" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
-        <v>32</v>
+      <c r="A5" s="46" t="s">
+        <v>29</v>
       </c>
       <c r="B5" s="30">
         <v>17640829</v>
@@ -1195,8 +1245,8 @@
       <c r="P5" s="31"/>
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
-        <v>33</v>
+      <c r="A6" s="47" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="30">
         <v>16173938</v>
@@ -1226,19 +1276,19 @@
       <c r="P6" s="31"/>
     </row>
     <row r="7" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="77">
+      <c r="A7" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="75">
         <v>4</v>
       </c>
-      <c r="C7" s="77">
+      <c r="C7" s="75">
         <v>4</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="75">
         <v>4</v>
       </c>
-      <c r="E7" s="77">
+      <c r="E7" s="75">
         <v>4</v>
       </c>
       <c r="F7" s="30"/>
@@ -1254,19 +1304,19 @@
       <c r="P7" s="31"/>
     </row>
     <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="78">
+      <c r="A8" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="76">
         <v>10000</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="76">
         <v>10000</v>
       </c>
-      <c r="D8" s="78">
+      <c r="D8" s="76">
         <v>8000</v>
       </c>
-      <c r="E8" s="78">
+      <c r="E8" s="76">
         <v>8000</v>
       </c>
       <c r="F8" s="30"/>
@@ -1281,49 +1331,50 @@
       <c r="O8" s="31"/>
       <c r="P8" s="31"/>
     </row>
-    <row r="9" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="49">
+    <row r="9" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="48">
         <v>2</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="48">
         <v>2</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="48">
         <v>2</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="48">
         <v>2</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="70"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
     </row>
     <row r="10" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="51">
-        <v>0</v>
-      </c>
-      <c r="C10" s="51">
-        <v>0</v>
-      </c>
-      <c r="D10" s="51">
-        <v>0</v>
-      </c>
-      <c r="E10" s="51">
+      <c r="A10" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="50">
+        <v>0</v>
+      </c>
+      <c r="C10" s="50">
+        <v>0</v>
+      </c>
+      <c r="D10" s="50">
+        <f>B75</f>
         <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E10" s="50">
+        <v>0</v>
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
@@ -1337,9 +1388,9 @@
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
     </row>
-    <row r="11" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="72" t="s">
-        <v>38</v>
+    <row r="11" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="70" t="s">
+        <v>35</v>
       </c>
       <c r="B11" s="17">
         <v>1650</v>
@@ -1353,21 +1404,21 @@
       <c r="E11" s="17">
         <v>1350</v>
       </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="70"/>
-      <c r="O11" s="70"/>
-      <c r="P11" s="70"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="68"/>
     </row>
     <row r="12" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="73" t="s">
-        <v>39</v>
+      <c r="A12" s="71" t="s">
+        <v>36</v>
       </c>
       <c r="B12" s="36">
         <v>3</v>
@@ -1381,18 +1432,18 @@
       <c r="E12" s="36">
         <v>5</v>
       </c>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
-        <v>40</v>
+      <c r="A13" s="46" t="s">
+        <v>37</v>
       </c>
       <c r="B13" s="34">
         <v>3.0000000000000001E-3</v>
@@ -1418,23 +1469,23 @@
       <c r="O13"/>
     </row>
     <row r="14" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="50">
-        <v>1</v>
-      </c>
-      <c r="C14" s="50">
-        <v>1</v>
-      </c>
-      <c r="D14" s="50">
-        <v>1</v>
-      </c>
-      <c r="E14" s="50">
-        <v>1</v>
+      <c r="A14" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="102">
+        <v>0.05</v>
+      </c>
+      <c r="C14" s="102">
+        <v>0.08</v>
+      </c>
+      <c r="D14" s="102">
+        <v>0.05</v>
+      </c>
+      <c r="E14" s="102">
+        <v>0.08</v>
       </c>
       <c r="F14" s="33"/>
-      <c r="G14" s="47"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
       <c r="J14" s="33"/>
@@ -1446,23 +1497,23 @@
       <c r="P14"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="50">
-        <v>1</v>
-      </c>
-      <c r="C15" s="50">
-        <v>1</v>
-      </c>
-      <c r="D15" s="50">
-        <v>1</v>
-      </c>
-      <c r="E15" s="50">
-        <v>1</v>
+      <c r="A15" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="102">
+        <v>1.23</v>
+      </c>
+      <c r="C15" s="102">
+        <v>1.08</v>
+      </c>
+      <c r="D15" s="102">
+        <v>1.23</v>
+      </c>
+      <c r="E15" s="102">
+        <v>1.08</v>
       </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="47"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
@@ -1473,33 +1524,33 @@
       <c r="O15"/>
     </row>
     <row r="16" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="73" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="75">
-        <v>0</v>
-      </c>
-      <c r="C16" s="75">
-        <v>0</v>
-      </c>
-      <c r="D16" s="75">
-        <v>0</v>
-      </c>
-      <c r="E16" s="75">
-        <v>0</v>
-      </c>
-      <c r="F16" s="76"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="76"/>
+      <c r="A16" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="73">
+        <v>0</v>
+      </c>
+      <c r="C16" s="73">
+        <v>0</v>
+      </c>
+      <c r="D16" s="73">
+        <v>0</v>
+      </c>
+      <c r="E16" s="73">
+        <v>0</v>
+      </c>
+      <c r="F16" s="74"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B17" s="35">
         <v>16750</v>
@@ -1516,7 +1567,7 @@
         <v>5700</v>
       </c>
       <c r="F17" s="35"/>
-      <c r="G17" s="47"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="35"/>
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
@@ -1528,7 +1579,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B18" s="35">
         <f>(B5+(C5+B6*B7)/2)/(B6+C6/2)</f>
@@ -1547,7 +1598,7 @@
         <v>3.5109478149000468</v>
       </c>
       <c r="F18" s="35"/>
-      <c r="G18" s="47"/>
+      <c r="G18" s="46"/>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
@@ -1559,7 +1610,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B19" s="35">
         <v>1.1000000000000001</v>
@@ -1574,7 +1625,7 @@
         <v>0.3</v>
       </c>
       <c r="F19" s="35"/>
-      <c r="G19" s="48"/>
+      <c r="G19" s="47"/>
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
@@ -1584,669 +1635,775 @@
       <c r="N19"/>
       <c r="O19"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="33">
-        <v>0</v>
-      </c>
-      <c r="C20" s="33">
-        <v>0</v>
-      </c>
-      <c r="D20" s="33">
-        <v>16</v>
-      </c>
-      <c r="E20" s="33">
-        <v>0</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="48"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20"/>
-      <c r="O20"/>
-    </row>
-    <row r="21" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="87" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="105">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E21" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="89">
-        <v>0.04</v>
-      </c>
-      <c r="G21" s="48"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21"/>
-      <c r="O21"/>
-    </row>
-    <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="39">
+    <row r="20" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="39">
         <f>B5/B6</f>
         <v>1.0906947337129647</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C20" s="39">
         <f>C5/C6</f>
         <v>2.8699385697067941</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D20" s="39">
         <f>D5/D6</f>
         <v>2.3844346304572381</v>
       </c>
-      <c r="E22" s="39">
+      <c r="E20" s="39">
         <f>E5/E6</f>
         <v>1.7226040825394728</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-    </row>
-    <row r="23" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="67" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="79" t="s">
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+    </row>
+    <row r="21" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="80">
+      <c r="C21" s="78">
         <f>C6/C8/C9</f>
         <v>404.93865</v>
       </c>
-      <c r="D23" s="79" t="s">
+      <c r="D21" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="80">
+      <c r="E21" s="78">
         <f>E6/E8/E9</f>
         <v>312.25968749999998</v>
       </c>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-    </row>
-    <row r="24" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="67" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="42">
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+    </row>
+    <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="42">
         <f>B19^2*B18/B13</f>
         <v>1228.751757325228</v>
       </c>
-      <c r="C24" s="42">
+      <c r="C22" s="42">
         <f>C19^2*C18/C13</f>
         <v>1228.751757325228</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D22" s="42">
         <f>D19^2*D18/D13</f>
         <v>105.3284344470014</v>
       </c>
-      <c r="E24" s="42">
+      <c r="E22" s="42">
         <f>E19^2*E18/E13</f>
         <v>105.3284344470014</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-    </row>
-    <row r="25" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="67" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="42">
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+    </row>
+    <row r="23" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="42">
         <f>B19*12.4*3600/PI()</f>
         <v>15630.288651168859</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C23" s="42">
         <f>C19*12.4*3600/PI()</f>
         <v>15630.288651168859</v>
       </c>
-      <c r="D25" s="42">
+      <c r="D23" s="42">
         <f>D19*12.4*3600/PI()</f>
         <v>4262.8059957733249</v>
       </c>
-      <c r="E25" s="42">
+      <c r="E23" s="42">
         <f>E19*12.4*3600/PI()</f>
         <v>4262.8059957733249</v>
       </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+    </row>
+    <row r="24" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="79" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="80">
+        <f>B22*B17/B23</f>
+        <v>1316.7761897767923</v>
+      </c>
+      <c r="C24" s="80">
+        <f>C22*C17/C23</f>
+        <v>1316.7761897767923</v>
+      </c>
+      <c r="D24" s="80">
+        <f>D22*D17/D23</f>
+        <v>140.8396434046474</v>
+      </c>
+      <c r="E24" s="80">
+        <f>E22*E17/E23</f>
+        <v>140.8396434046474</v>
+      </c>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="80"/>
+    </row>
+    <row r="25" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="78">
+        <f>C22*C7/2*C8/C23</f>
+        <v>1572.2700773454237</v>
+      </c>
+      <c r="D25" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="78">
+        <f>E22*E7/2*E8/E23</f>
+        <v>395.33934990778221</v>
+      </c>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
       <c r="L25" s="42"/>
       <c r="M25" s="42"/>
     </row>
-    <row r="26" spans="1:16" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="81" t="s">
+    <row r="26" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="78">
+        <f>C19^2*C20/C13*C7/2*C8/C23</f>
+        <v>1481.1522878628059</v>
+      </c>
+      <c r="D26" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="78">
+        <f>E19^2*E20/E13*E7/2*E8/E23</f>
+        <v>193.96847063619333</v>
+      </c>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+    </row>
+    <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="44">
+        <f>PI()*C21/12.4/3600</f>
+        <v>2.8498035125326355E-2</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="44">
+        <f>PI()*E21/12.4/3600</f>
+        <v>2.1975643823078955E-2</v>
+      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+    </row>
+    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="44">
+        <f>C27^2*C20/C13*C9</f>
+        <v>1.5538574582377387</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="44">
+        <f>E27^2*E20/E13*E9</f>
+        <v>0.55459688776460658</v>
+      </c>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="44"/>
+    </row>
+    <row r="29" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="82">
-        <f>B24*B17/B25</f>
-        <v>1316.7761897767923</v>
-      </c>
-      <c r="C26" s="82">
-        <f>C24*C17/C25</f>
-        <v>1316.7761897767923</v>
-      </c>
-      <c r="D26" s="82">
-        <f>D24*D17/D25</f>
-        <v>140.8396434046474</v>
-      </c>
-      <c r="E26" s="82">
-        <f>E24*E17/E25</f>
-        <v>140.8396434046474</v>
-      </c>
-      <c r="F26" s="82"/>
-      <c r="G26" s="82"/>
-      <c r="H26" s="82"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="82"/>
-      <c r="K26" s="82"/>
-      <c r="L26" s="82"/>
-      <c r="M26" s="82"/>
-    </row>
-    <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="67" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="79" t="s">
+      <c r="B29" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="80">
-        <f>C24*C7/2*C8/C25</f>
-        <v>1572.2700773454237</v>
-      </c>
-      <c r="D27" s="79" t="s">
+      <c r="C29" s="82">
+        <f>C28*C7/2*C8/C21</f>
+        <v>76.745327137221338</v>
+      </c>
+      <c r="D29" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="80">
-        <f>E24*E7/2*E8/E25</f>
-        <v>395.33934990778221</v>
-      </c>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-    </row>
-    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="80">
-        <f>C19^2*C22/C13*C7/2*C8/C25</f>
-        <v>1481.1522878628059</v>
-      </c>
-      <c r="D28" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="80">
-        <f>E19^2*E22/E13*E7/2*E8/E25</f>
-        <v>193.96847063619333</v>
-      </c>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-    </row>
-    <row r="29" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="67" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="44">
-        <f>PI()*C23/12.4/3600</f>
-        <v>2.8498035125326355E-2</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="44">
-        <f>PI()*E23/12.4/3600</f>
-        <v>2.1975643823078955E-2</v>
-      </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-    </row>
-    <row r="30" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="44">
-        <f>C29^2*C22/C13*C9</f>
-        <v>1.5538574582377387</v>
-      </c>
-      <c r="D30" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="44">
-        <f>E29^2*E22/E13*E9</f>
-        <v>0.55459688776460658</v>
-      </c>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="44"/>
-    </row>
-    <row r="31" spans="1:16" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="83" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="84">
-        <f>C30*C7/2*C8/C23</f>
-        <v>76.745327137221338</v>
-      </c>
-      <c r="D31" s="83" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="84">
-        <f>E30*E7/2*E8/E23</f>
+      <c r="E29" s="82">
+        <f>E28*E7/2*E8/E21</f>
         <v>28.417213490722222</v>
       </c>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="86"/>
-      <c r="J31" s="85"/>
-      <c r="K31" s="85"/>
-      <c r="L31" s="86"/>
-      <c r="M31" s="86"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B32" s="8"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="5"/>
+      <c r="F29" s="83"/>
+      <c r="G29" s="83"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="83"/>
+      <c r="K29" s="83"/>
+      <c r="L29" s="84"/>
+      <c r="M29" s="84"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="8"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="15"/>
+      <c r="P31" s="14"/>
+    </row>
+    <row r="32" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
     </row>
     <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="15"/>
-      <c r="P33" s="14"/>
-    </row>
-    <row r="34" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="5">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
+      <c r="B35" s="8">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" s="5">
-        <v>6.1</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="8">
-        <v>0.1</v>
+      <c r="B37" s="5">
+        <v>2650</v>
       </c>
     </row>
     <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="5">
-        <v>1025</v>
+      <c r="B38" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" s="5">
-        <v>2650</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="10">
-        <v>2E-3</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>7</v>
+      <c r="B40" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="5">
-        <v>2</v>
+      <c r="B41" s="5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" s="53"/>
-      <c r="B45" s="52"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
-    </row>
-    <row r="46" spans="1:17" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="54" t="s">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" s="52"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+    </row>
+    <row r="44" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="D46" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="E46" s="56"/>
+      <c r="B44" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="55"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="56"/>
+      <c r="L44" s="57"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="58"/>
+      <c r="O44" s="58"/>
+    </row>
+    <row r="45" spans="1:17" s="59" customFormat="1" ht="87.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="61"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="57"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="58"/>
+      <c r="O45" s="58"/>
+    </row>
+    <row r="46" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="60"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
       <c r="F46" s="57"/>
       <c r="G46" s="57"/>
       <c r="H46" s="57"/>
-      <c r="I46" s="57"/>
+      <c r="I46" s="64"/>
       <c r="J46" s="57"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="59"/>
-      <c r="N46" s="59"/>
-      <c r="O46" s="59"/>
-    </row>
-    <row r="47" spans="1:17" s="60" customFormat="1" ht="100" x14ac:dyDescent="0.3">
-      <c r="A47" s="61" t="s">
+      <c r="L46" s="57"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="58"/>
+    </row>
+    <row r="47" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="60"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="64"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="58"/>
+    </row>
+    <row r="48" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="60"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="64"/>
+      <c r="L48" s="57"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
+    </row>
+    <row r="49" spans="1:15" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="60"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="64"/>
+      <c r="L49" s="57"/>
+      <c r="M49" s="58"/>
+      <c r="N49" s="58"/>
+      <c r="O49" s="58"/>
+    </row>
+    <row r="50" spans="1:15" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="60"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="64"/>
+      <c r="L50" s="57"/>
+      <c r="M50" s="58"/>
+      <c r="N50" s="58"/>
+      <c r="O50" s="58"/>
+    </row>
+    <row r="51" spans="1:15" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="60"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="57"/>
+      <c r="M51" s="58"/>
+      <c r="N51" s="58"/>
+      <c r="O51" s="58"/>
+    </row>
+    <row r="52" spans="1:15" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="60"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="64"/>
+      <c r="G52" s="64"/>
+      <c r="H52" s="64"/>
+      <c r="I52" s="64"/>
+      <c r="J52" s="64"/>
+      <c r="K52" s="64"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="58"/>
+      <c r="N52" s="58"/>
+      <c r="O52" s="58"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="65"/>
+      <c r="C54" s="49"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="49">
+        <v>2</v>
+      </c>
+      <c r="C55" s="49"/>
+      <c r="D55" s="49"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A56" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="49">
+        <v>2E-3</v>
+      </c>
+      <c r="C56" s="49"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="101">
+        <v>2E-3</v>
+      </c>
+      <c r="C57" s="49"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="49">
+        <v>1</v>
+      </c>
+      <c r="C58" s="49"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="98">
+        <v>0.15</v>
+      </c>
+      <c r="C59" s="49"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" s="98">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="C60" s="49"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="98">
+        <v>12.2</v>
+      </c>
+      <c r="C61" s="49"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="32">
+        <v>1</v>
+      </c>
+      <c r="C62" s="49"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A63" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="65"/>
+      <c r="C63" s="49"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A64" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="32">
+        <v>0.04</v>
+      </c>
+      <c r="C64" s="49"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="32">
+        <v>0.04</v>
+      </c>
+      <c r="C65" s="49"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66" s="32">
+        <v>9000</v>
+      </c>
+      <c r="C66" s="49"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B67" s="32">
         <v>10</v>
       </c>
-      <c r="B47" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="62"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="57"/>
-      <c r="J47" s="57"/>
-      <c r="K47" s="57"/>
-      <c r="L47" s="58"/>
-      <c r="M47" s="59"/>
-      <c r="N47" s="59"/>
-      <c r="O47" s="59"/>
-    </row>
-    <row r="48" spans="1:17" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="66"/>
-      <c r="J48" s="58"/>
-      <c r="L48" s="58"/>
-      <c r="M48" s="59"/>
-      <c r="N48" s="59"/>
-      <c r="O48" s="59"/>
-    </row>
-    <row r="49" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="64" t="s">
+      <c r="C67" s="49"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B68" s="32">
+        <v>10</v>
+      </c>
+      <c r="C68" s="49"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="65"/>
+      <c r="C69" s="49"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="49">
+        <v>1</v>
+      </c>
+      <c r="C70" s="49"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="32">
+        <v>300</v>
+      </c>
+      <c r="C71" s="49"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B72" s="32">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="B73" s="65"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" s="49">
         <v>16</v>
       </c>
-      <c r="B49" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="66"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="58"/>
-      <c r="M49" s="59"/>
-      <c r="N49" s="59"/>
-      <c r="O49" s="59"/>
-    </row>
-    <row r="50" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="64" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="58"/>
-      <c r="L50" s="58"/>
-      <c r="M50" s="59"/>
-      <c r="N50" s="59"/>
-      <c r="O50" s="59"/>
-    </row>
-    <row r="51" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="64" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="66"/>
-      <c r="J51" s="66"/>
-      <c r="L51" s="58"/>
-      <c r="M51" s="59"/>
-      <c r="N51" s="59"/>
-      <c r="O51" s="59"/>
-    </row>
-    <row r="52" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="66"/>
-      <c r="J52" s="66"/>
-      <c r="L52" s="58"/>
-      <c r="M52" s="59"/>
-      <c r="N52" s="59"/>
-      <c r="O52" s="59"/>
-    </row>
-    <row r="53" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="61"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="66"/>
-      <c r="J53" s="66"/>
-      <c r="L53" s="58"/>
-      <c r="M53" s="59"/>
-      <c r="N53" s="59"/>
-      <c r="O53" s="59"/>
-    </row>
-    <row r="54" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="64" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="61"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
-      <c r="K54" s="58"/>
-      <c r="L54" s="58"/>
-      <c r="M54" s="59"/>
-      <c r="N54" s="59"/>
-      <c r="O54" s="59"/>
-    </row>
-    <row r="55" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="61"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="66"/>
-      <c r="G55" s="66"/>
-      <c r="H55" s="66"/>
-      <c r="I55" s="66"/>
-      <c r="J55" s="66"/>
-      <c r="K55" s="66"/>
-      <c r="L55" s="58"/>
-      <c r="M55" s="59"/>
-      <c r="N55" s="59"/>
-      <c r="O55" s="59"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="20"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" s="32">
+        <v>5.0000000000000001E-3</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2262,20 +2419,20 @@
   <dimension ref="A1:V80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="A6:E80"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.08984375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" style="93" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" style="96" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" style="93" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="96" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" style="93" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" style="96" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" style="93" customWidth="1"/>
-    <col min="9" max="9" width="12.7265625" style="96" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="88" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="91" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="88" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="91" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" style="88" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="91" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="88" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" style="91" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
@@ -2285,199 +2442,201 @@
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="99" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:22" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="92" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1"/>
+    </row>
+    <row r="2" spans="1:22" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="93" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:22" s="86" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="85" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="100" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-    </row>
-    <row r="2" spans="1:22" s="99" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="100" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-    </row>
-    <row r="3" spans="1:22" s="91" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="90" t="s">
+      <c r="G3" s="100"/>
+      <c r="H3" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="106" t="s">
+      <c r="I3" s="100"/>
+    </row>
+    <row r="4" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="95"/>
+      <c r="B4" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106" t="s">
+      <c r="D4" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="89" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="106"/>
-    </row>
-    <row r="4" spans="1:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="102"/>
-      <c r="B4" s="94" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="94" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="94" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="94" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="94" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="94" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="94" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="94" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="101" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="94" t="s">
-        <v>65</v>
+      <c r="C5" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="89" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="101">
+      <c r="A6" s="94">
         <v>1926</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="92">
-        <v>0</v>
-      </c>
-      <c r="E6" s="95"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="93">
+      <c r="B6" s="87"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="87">
+        <v>0</v>
+      </c>
+      <c r="E6" s="90"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="88">
         <v>420000</v>
       </c>
-      <c r="I6" s="96">
+      <c r="I6" s="91">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="101">
+      <c r="A7" s="94">
         <v>1927</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="103">
+      <c r="B7" s="87"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="96">
         <v>420000</v>
       </c>
-      <c r="F7" s="92"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="93">
+      <c r="F7" s="87"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="88">
         <v>-2098785</v>
       </c>
-      <c r="I7" s="96">
+      <c r="I7" s="91">
         <v>-667500</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="101">
+      <c r="A8" s="94">
         <v>1928</v>
       </c>
-      <c r="B8" s="92"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="103">
+      <c r="B8" s="87"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="96">
         <v>420000</v>
       </c>
-      <c r="F8" s="92"/>
-      <c r="G8" s="95"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="90"/>
     </row>
     <row r="9" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="101">
+      <c r="A9" s="94">
         <v>1929</v>
       </c>
-      <c r="B9" s="92"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="103">
+      <c r="B9" s="87"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="96">
         <v>420000</v>
       </c>
-      <c r="F9" s="92"/>
-      <c r="G9" s="95"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="90"/>
     </row>
     <row r="10" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="101">
+      <c r="A10" s="94">
         <v>1930</v>
       </c>
-      <c r="D10" s="103">
+      <c r="D10" s="96">
         <v>420000</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="101">
+      <c r="A11" s="94">
         <v>1931</v>
       </c>
-      <c r="D11" s="93">
+      <c r="D11" s="88">
         <v>965050</v>
       </c>
-      <c r="E11" s="96">
+      <c r="E11" s="91">
         <v>710743</v>
       </c>
-      <c r="H11" s="93">
+      <c r="H11" s="88">
         <v>-2305143</v>
       </c>
-      <c r="I11" s="96">
+      <c r="I11" s="91">
         <v>-1147381</v>
       </c>
       <c r="N11" s="28"/>
     </row>
     <row r="12" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="101">
+      <c r="A12" s="94">
         <v>1932</v>
       </c>
-      <c r="D12" s="103">
+      <c r="D12" s="96">
         <v>420000</v>
       </c>
       <c r="M12" s="18"/>
@@ -2492,10 +2651,10 @@
       <c r="V12" s="19"/>
     </row>
     <row r="13" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="101">
+      <c r="A13" s="94">
         <v>1933</v>
       </c>
-      <c r="D13" s="103">
+      <c r="D13" s="96">
         <v>420000</v>
       </c>
       <c r="M13" s="18"/>
@@ -2510,10 +2669,10 @@
       <c r="V13" s="19"/>
     </row>
     <row r="14" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="101">
+      <c r="A14" s="94">
         <v>1934</v>
       </c>
-      <c r="D14" s="103">
+      <c r="D14" s="96">
         <v>420000</v>
       </c>
       <c r="M14" s="19"/>
@@ -2527,10 +2686,10 @@
       <c r="U14" s="9"/>
     </row>
     <row r="15" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="101">
+      <c r="A15" s="94">
         <v>1935</v>
       </c>
-      <c r="D15" s="103">
+      <c r="D15" s="96">
         <v>420000</v>
       </c>
       <c r="M15" s="19"/>
@@ -2544,10 +2703,10 @@
       <c r="U15" s="9"/>
     </row>
     <row r="16" spans="1:22" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="101">
+      <c r="A16" s="94">
         <v>1936</v>
       </c>
-      <c r="D16" s="103">
+      <c r="D16" s="96">
         <v>420000</v>
       </c>
       <c r="M16" s="19"/>
@@ -2561,10 +2720,10 @@
       <c r="U16" s="9"/>
     </row>
     <row r="17" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="101">
+      <c r="A17" s="94">
         <v>1937</v>
       </c>
-      <c r="D17" s="103">
+      <c r="D17" s="96">
         <v>420000</v>
       </c>
       <c r="M17" s="19"/>
@@ -2578,13 +2737,13 @@
       <c r="U17" s="9"/>
     </row>
     <row r="18" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="101">
+      <c r="A18" s="94">
         <v>1938</v>
       </c>
-      <c r="D18" s="104">
+      <c r="D18" s="97">
         <v>920000</v>
       </c>
-      <c r="E18" s="96">
+      <c r="E18" s="91">
         <v>0</v>
       </c>
       <c r="M18" s="19"/>
@@ -2598,10 +2757,10 @@
       <c r="U18" s="9"/>
     </row>
     <row r="19" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="101">
+      <c r="A19" s="94">
         <v>1939</v>
       </c>
-      <c r="D19" s="103">
+      <c r="D19" s="96">
         <v>370000</v>
       </c>
       <c r="M19" s="19"/>
@@ -2615,19 +2774,19 @@
       <c r="U19" s="9"/>
     </row>
     <row r="20" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="101">
+      <c r="A20" s="94">
         <v>1940</v>
       </c>
-      <c r="D20" s="103">
+      <c r="D20" s="96">
         <v>370000</v>
       </c>
       <c r="N20" s="29"/>
     </row>
     <row r="21" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="101">
+      <c r="A21" s="94">
         <v>1941</v>
       </c>
-      <c r="D21" s="103">
+      <c r="D21" s="96">
         <v>370000</v>
       </c>
       <c r="M21" s="24"/>
@@ -2640,10 +2799,10 @@
       <c r="T21" s="5"/>
     </row>
     <row r="22" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="101">
+      <c r="A22" s="94">
         <v>1942</v>
       </c>
-      <c r="D22" s="103">
+      <c r="D22" s="96">
         <v>370000</v>
       </c>
       <c r="M22" s="23"/>
@@ -2656,10 +2815,10 @@
       <c r="T22" s="5"/>
     </row>
     <row r="23" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="101">
+      <c r="A23" s="94">
         <v>1943</v>
       </c>
-      <c r="D23" s="103">
+      <c r="D23" s="96">
         <v>370000</v>
       </c>
       <c r="M23" s="23"/>
@@ -2672,10 +2831,10 @@
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="101">
+      <c r="A24" s="94">
         <v>1944</v>
       </c>
-      <c r="D24" s="103">
+      <c r="D24" s="96">
         <v>370000</v>
       </c>
       <c r="M24" s="23"/>
@@ -2688,10 +2847,10 @@
       <c r="T24" s="5"/>
     </row>
     <row r="25" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="101">
+      <c r="A25" s="94">
         <v>1945</v>
       </c>
-      <c r="D25" s="103">
+      <c r="D25" s="96">
         <v>370000</v>
       </c>
       <c r="M25" s="23"/>
@@ -2704,10 +2863,10 @@
       <c r="T25" s="5"/>
     </row>
     <row r="26" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A26" s="101">
+      <c r="A26" s="94">
         <v>1946</v>
       </c>
-      <c r="D26" s="103">
+      <c r="D26" s="96">
         <v>370000</v>
       </c>
       <c r="M26" s="23"/>
@@ -2720,10 +2879,10 @@
       <c r="T26" s="5"/>
     </row>
     <row r="27" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="101">
+      <c r="A27" s="94">
         <v>1947</v>
       </c>
-      <c r="D27" s="103">
+      <c r="D27" s="96">
         <v>370000</v>
       </c>
       <c r="M27" s="23"/>
@@ -2736,461 +2895,461 @@
       <c r="T27" s="5"/>
     </row>
     <row r="28" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="101">
+      <c r="A28" s="94">
         <v>1948</v>
       </c>
-      <c r="D28" s="103">
+      <c r="D28" s="96">
         <v>370000</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A29" s="101">
+      <c r="A29" s="94">
         <v>1949</v>
       </c>
-      <c r="D29" s="103">
+      <c r="D29" s="96">
         <v>370000</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A30" s="101">
+      <c r="A30" s="94">
         <v>1950</v>
       </c>
-      <c r="D30" s="103">
+      <c r="D30" s="96">
         <v>270000</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A31" s="101">
+      <c r="A31" s="94">
         <v>1951</v>
       </c>
-      <c r="D31" s="103">
+      <c r="D31" s="96">
         <v>270000</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="101">
+      <c r="A32" s="94">
         <v>1952</v>
       </c>
-      <c r="D32" s="103">
+      <c r="D32" s="96">
         <v>270000</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A33" s="101">
+      <c r="A33" s="94">
         <v>1953</v>
       </c>
-      <c r="D33" s="103">
+      <c r="D33" s="96">
         <v>270000</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A34" s="101">
+      <c r="A34" s="94">
         <v>1954</v>
       </c>
-      <c r="D34" s="103">
+      <c r="D34" s="96">
         <v>270000</v>
       </c>
       <c r="N34" s="11"/>
     </row>
     <row r="35" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A35" s="101">
+      <c r="A35" s="94">
         <v>1955</v>
       </c>
-      <c r="D35" s="103">
+      <c r="D35" s="96">
         <v>270000</v>
       </c>
       <c r="N35" s="11"/>
     </row>
     <row r="36" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A36" s="101">
+      <c r="A36" s="94">
         <v>1956</v>
       </c>
-      <c r="D36" s="103">
+      <c r="D36" s="96">
         <v>270000</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A37" s="101">
+      <c r="A37" s="94">
         <v>1957</v>
       </c>
-      <c r="D37" s="103">
+      <c r="D37" s="96">
         <v>270000</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A38" s="101">
+      <c r="A38" s="94">
         <v>1958</v>
       </c>
-      <c r="D38" s="103">
+      <c r="D38" s="96">
         <v>270000</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A39" s="101">
+      <c r="A39" s="94">
         <v>1959</v>
       </c>
-      <c r="D39" s="103">
+      <c r="D39" s="96">
         <v>270000</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A40" s="101">
+      <c r="A40" s="94">
         <v>1960</v>
       </c>
-      <c r="D40" s="103">
+      <c r="D40" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A41" s="101">
+      <c r="A41" s="94">
         <v>1961</v>
       </c>
-      <c r="D41" s="103">
-        <v>280000</v>
-      </c>
-      <c r="H41" s="93">
+      <c r="D41" s="96">
+        <v>280000</v>
+      </c>
+      <c r="H41" s="88">
         <v>-1523786</v>
       </c>
-      <c r="I41" s="96">
+      <c r="I41" s="91">
         <v>-412500</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A42" s="101">
+      <c r="A42" s="94">
         <v>1962</v>
       </c>
-      <c r="D42" s="103">
+      <c r="D42" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A43" s="101">
+      <c r="A43" s="94">
         <v>1963</v>
       </c>
-      <c r="D43" s="103">
+      <c r="D43" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A44" s="101">
+      <c r="A44" s="94">
         <v>1964</v>
       </c>
-      <c r="D44" s="103">
+      <c r="D44" s="96">
         <v>300000</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="101">
+      <c r="A45" s="94">
         <v>1965</v>
       </c>
-      <c r="B45" s="93">
+      <c r="B45" s="88">
         <v>44506</v>
       </c>
-      <c r="C45" s="96">
+      <c r="C45" s="91">
         <v>48739</v>
       </c>
-      <c r="D45" s="93">
+      <c r="D45" s="88">
         <v>7636675</v>
       </c>
-      <c r="E45" s="96">
+      <c r="E45" s="91">
         <v>343245</v>
       </c>
-      <c r="F45" s="93">
+      <c r="F45" s="88">
         <v>-2695096</v>
       </c>
-      <c r="G45" s="96">
+      <c r="G45" s="91">
         <v>-1861535</v>
       </c>
-      <c r="H45" s="93">
+      <c r="H45" s="88">
         <v>-2830178</v>
       </c>
-      <c r="I45" s="96">
+      <c r="I45" s="91">
         <v>-1371379</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A46" s="101">
+      <c r="A46" s="94">
         <v>1966</v>
       </c>
-      <c r="D46" s="103">
+      <c r="D46" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A47" s="101">
+      <c r="A47" s="94">
         <v>1967</v>
       </c>
-      <c r="D47" s="103">
+      <c r="D47" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A48" s="101">
+      <c r="A48" s="94">
         <v>1968</v>
       </c>
-      <c r="D48" s="103">
+      <c r="D48" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A49" s="101">
+      <c r="A49" s="94">
         <v>1969</v>
       </c>
-      <c r="D49" s="103">
+      <c r="D49" s="96">
         <v>780000</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A50" s="101">
+      <c r="A50" s="94">
         <v>1970</v>
       </c>
-      <c r="D50" s="103">
+      <c r="D50" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A51" s="101">
+      <c r="A51" s="94">
         <v>1971</v>
       </c>
-      <c r="D51" s="103">
+      <c r="D51" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A52" s="101">
+      <c r="A52" s="94">
         <v>1972</v>
       </c>
-      <c r="D52" s="103">
+      <c r="D52" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A53" s="101">
+      <c r="A53" s="94">
         <v>1973</v>
       </c>
-      <c r="D53" s="103">
+      <c r="D53" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A54" s="101">
+      <c r="A54" s="94">
         <v>1974</v>
       </c>
-      <c r="D54" s="103">
+      <c r="D54" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A55" s="101">
+      <c r="A55" s="94">
         <v>1975</v>
       </c>
-      <c r="D55" s="103">
+      <c r="D55" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A56" s="101">
+      <c r="A56" s="94">
         <v>1976</v>
       </c>
-      <c r="D56" s="103">
+      <c r="D56" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A57" s="101">
+      <c r="A57" s="94">
         <v>1977</v>
       </c>
-      <c r="D57" s="103">
+      <c r="D57" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A58" s="101">
+      <c r="A58" s="94">
         <v>1978</v>
       </c>
-      <c r="D58" s="103">
+      <c r="D58" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A59" s="101">
+      <c r="A59" s="94">
         <v>1979</v>
       </c>
-      <c r="D59" s="103">
+      <c r="D59" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A60" s="101">
+      <c r="A60" s="94">
         <v>1980</v>
       </c>
-      <c r="D60" s="103">
+      <c r="D60" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A61" s="101">
+      <c r="A61" s="94">
         <v>1981</v>
       </c>
-      <c r="D61" s="103">
+      <c r="D61" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A62" s="101">
+      <c r="A62" s="94">
         <v>1982</v>
       </c>
-      <c r="D62" s="103">
+      <c r="D62" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A63" s="101">
+      <c r="A63" s="94">
         <v>1983</v>
       </c>
-      <c r="D63" s="103">
+      <c r="D63" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A64" s="101">
+      <c r="A64" s="94">
         <v>1984</v>
       </c>
-      <c r="D64" s="103">
+      <c r="D64" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A65" s="101">
+      <c r="A65" s="94">
         <v>1985</v>
       </c>
-      <c r="D65" s="103">
+      <c r="D65" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A66" s="101">
+      <c r="A66" s="94">
         <v>1986</v>
       </c>
-      <c r="D66" s="103">
+      <c r="D66" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A67" s="101">
+      <c r="A67" s="94">
         <v>1987</v>
       </c>
-      <c r="D67" s="103">
+      <c r="D67" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A68" s="101">
+      <c r="A68" s="94">
         <v>1988</v>
       </c>
-      <c r="D68" s="103">
+      <c r="D68" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A69" s="101">
+      <c r="A69" s="94">
         <v>1989</v>
       </c>
-      <c r="D69" s="103">
+      <c r="D69" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A70" s="101">
+      <c r="A70" s="94">
         <v>1990</v>
       </c>
-      <c r="D70" s="103">
+      <c r="D70" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A71" s="101">
+      <c r="A71" s="94">
         <v>1991</v>
       </c>
-      <c r="D71" s="103">
+      <c r="D71" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A72" s="101">
+      <c r="A72" s="94">
         <v>1992</v>
       </c>
-      <c r="D72" s="103">
+      <c r="D72" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A73" s="101">
+      <c r="A73" s="94">
         <v>1993</v>
       </c>
-      <c r="D73" s="103">
+      <c r="D73" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A74" s="101">
+      <c r="A74" s="94">
         <v>1994</v>
       </c>
-      <c r="D74" s="103">
+      <c r="D74" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="101">
+      <c r="A75" s="94">
         <v>1995</v>
       </c>
-      <c r="D75" s="93">
+      <c r="D75" s="88">
         <v>3280000</v>
       </c>
-      <c r="E75" s="96">
+      <c r="E75" s="91">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A76" s="101">
+      <c r="A76" s="94">
         <v>1996</v>
       </c>
-      <c r="D76" s="103">
+      <c r="D76" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A77" s="101">
+      <c r="A77" s="94">
         <v>1997</v>
       </c>
-      <c r="D77" s="103">
+      <c r="D77" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="101">
+      <c r="A78" s="94">
         <v>1998</v>
       </c>
-      <c r="D78" s="93">
+      <c r="D78" s="88">
         <v>2280000</v>
       </c>
-      <c r="E78" s="96">
+      <c r="E78" s="91">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A79" s="101">
+      <c r="A79" s="94">
         <v>1999</v>
       </c>
-      <c r="D79" s="103">
+      <c r="D79" s="96">
         <v>280000</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A80" s="101">
+      <c r="A80" s="94">
         <v>2000</v>
       </c>
-      <c r="D80" s="103">
+      <c r="D80" s="96">
         <v>280000</v>
       </c>
     </row>
@@ -3220,13 +3379,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5164,7 +5323,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5181,31 +5340,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>